<commit_message>
slight tweak plate layout sample labels
</commit_message>
<xml_diff>
--- a/example_data/example_platelayout.xlsx
+++ b/example_data/example_platelayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruybal.s/Documents/covid-19/covidClassifyR/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA853528-4E8F-564A-8CCE-78BD8BBC43D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4551D8A7-3BB2-EC4D-8F17-F4F920AF4322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>Blank2</t>
   </si>
   <si>
-    <t>Blank3</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>ABC083</t>
+  </si>
+  <si>
+    <t>ABC084</t>
   </si>
 </sst>
 </file>
@@ -755,13 +755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -813,37 +814,37 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13">

</xml_diff>